<commit_message>
inheritance update finish, datamap broken
</commit_message>
<xml_diff>
--- a/Resources/TestCaseSheet.xlsx
+++ b/Resources/TestCaseSheet.xlsx
@@ -34,12 +34,6 @@
     <t>TEST_DATA</t>
   </si>
   <si>
-    <t>EnrollMember</t>
-  </si>
-  <si>
-    <t>MemberPayment</t>
-  </si>
-  <si>
     <t>MEM001;MEM001</t>
   </si>
   <si>
@@ -50,6 +44,12 @@
   </si>
   <si>
     <t>MEM005,MEM006,TXN002;MEM006,MEM005,TXN001</t>
+  </si>
+  <si>
+    <t>MemberPayments</t>
+  </si>
+  <si>
+    <t>EnrollNewMember</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,30 +453,30 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dataprovider test control added clean
</commit_message>
<xml_diff>
--- a/Resources/TestCaseSheet.xlsx
+++ b/Resources/TestCaseSheet.xlsx
@@ -34,9 +34,6 @@
     <t>TEST_DATA</t>
   </si>
   <si>
-    <t>MEM001;MEM001</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>EnrollNewMember</t>
+  </si>
+  <si>
+    <t>MEM004,MEM001;MEM004,MEM001</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,16 +453,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -473,10 +473,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>